<commit_message>
partial done with merge.ipynb
</commit_message>
<xml_diff>
--- a/assets/metadata/Wrds-Refinitiv fields.xlsx
+++ b/assets/metadata/Wrds-Refinitiv fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tifannyh\Documents\nBox\Tifanny\Database\Refinitiv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\DataMining\assets\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547B747B-AAB4-4066-8244-AC66D585A10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A6355D-1A2D-4449-8D62-DDD160B45EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13092" xr2:uid="{E198CB92-F244-4729-ACF6-B0F66D066286}"/>
+    <workbookView xWindow="-16305" yWindow="0" windowWidth="16410" windowHeight="14505" xr2:uid="{E198CB92-F244-4729-ACF6-B0F66D066286}"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="706">
   <si>
     <t>Var Fields</t>
   </si>
@@ -870,9 +870,6 @@
   </si>
   <si>
     <t>Preferred Stock - Liquidating Value</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>[wrds] Similar value to that of PSTK. 
@@ -2168,13 +2165,16 @@
   </si>
   <si>
     <t>if be&gt;0 then ptb=mktcap/be; else ptb=.;</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2333,7 +2333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2438,6 +2438,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2756,13 +2759,13 @@
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E58" sqref="E58"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I49" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48" style="33" customWidth="1"/>
@@ -2776,7 +2779,7 @@
     <col min="10" max="10" width="53.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2808,12 +2811,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="30" customFormat="1">
+    <row r="2" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
+      <c r="C2" s="26" t="s">
+        <v>705</v>
+      </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
@@ -2822,12 +2827,14 @@
       <c r="I2" s="29"/>
       <c r="J2" s="31"/>
     </row>
-    <row r="3" spans="1:10" s="30" customFormat="1">
+    <row r="3" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="C3" s="26" t="s">
+        <v>705</v>
+      </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
@@ -2836,12 +2843,14 @@
       <c r="I3" s="29"/>
       <c r="J3" s="27"/>
     </row>
-    <row r="4" spans="1:10" s="30" customFormat="1">
+    <row r="4" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="C4" s="26" t="s">
+        <v>705</v>
+      </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
@@ -2850,14 +2859,16 @@
       <c r="I4" s="29"/>
       <c r="J4" s="27"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="41" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -2874,14 +2885,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="41" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2898,14 +2911,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="41" t="s">
+        <v>25</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -2922,14 +2937,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="41" t="s">
+        <v>31</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -2946,14 +2963,16 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -2970,14 +2989,16 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="41" t="s">
+        <v>43</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -2994,14 +3015,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="41" t="s">
+        <v>49</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -3018,14 +3041,16 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="41" t="s">
+        <v>55</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -3042,14 +3067,16 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>61</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="41" t="s">
+        <v>61</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -3066,14 +3093,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1">
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>67</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -3090,14 +3119,16 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>73</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="41" t="s">
+        <v>73</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -3114,14 +3145,16 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>79</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="41" t="s">
+        <v>79</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -3138,14 +3171,16 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="55.9" customHeight="1">
+    <row r="17" spans="1:11" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>85</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="41" t="s">
+        <v>85</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -3162,14 +3197,16 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="41" t="s">
+        <v>91</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -3186,14 +3223,16 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="55.15">
+    <row r="19" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="41" t="s">
+        <v>97</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -3210,14 +3249,16 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>103</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="41" t="s">
+        <v>103</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -3234,14 +3275,16 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>109</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="41" t="s">
+        <v>109</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -3258,14 +3301,16 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="41.45">
+    <row r="22" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>115</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="41" t="s">
+        <v>115</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -3281,14 +3326,16 @@
       </c>
       <c r="K22" s="13"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>120</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="41" t="s">
+        <v>120</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -3305,14 +3352,16 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>125</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="41" t="s">
+        <v>125</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -3329,14 +3378,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>131</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="41" t="s">
+        <v>131</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -3353,14 +3404,16 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>137</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="41" t="s">
+        <v>137</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -3377,14 +3430,16 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>143</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="41" t="s">
+        <v>143</v>
+      </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -3401,14 +3456,16 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="55.15">
+    <row r="28" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>149</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="41" t="s">
+        <v>149</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -3423,14 +3480,16 @@
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>154</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="41" t="s">
+        <v>154</v>
+      </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -3447,14 +3506,16 @@
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>160</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="41" t="s">
+        <v>160</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -3471,14 +3532,16 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>162</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="41" t="s">
+        <v>162</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -3495,14 +3558,16 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>168</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="41" t="s">
+        <v>168</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -3519,14 +3584,16 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>174</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="41" t="s">
+        <v>174</v>
+      </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -3543,14 +3610,16 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="41" t="s">
+        <v>180</v>
+      </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -3567,14 +3636,16 @@
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>186</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="41" t="s">
+        <v>186</v>
+      </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -3591,14 +3662,16 @@
         <v>191</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>192</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="C36" s="41" t="s">
+        <v>192</v>
+      </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -3615,14 +3688,16 @@
         <v>191</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>194</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="41" t="s">
+        <v>194</v>
+      </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -3640,14 +3715,16 @@
       </c>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>200</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C38" s="4"/>
+      <c r="C38" s="41" t="s">
+        <v>200</v>
+      </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -3664,14 +3741,16 @@
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>206</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C39" s="4"/>
+      <c r="C39" s="41" t="s">
+        <v>206</v>
+      </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -3688,14 +3767,16 @@
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="13" customFormat="1">
+    <row r="40" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>212</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C40" s="4"/>
+      <c r="C40" s="41" t="s">
+        <v>212</v>
+      </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -3713,14 +3794,16 @@
       </c>
       <c r="K40"/>
     </row>
-    <row r="41" spans="1:11" s="13" customFormat="1">
+    <row r="41" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>218</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C41" s="4"/>
+      <c r="C41" s="41" t="s">
+        <v>218</v>
+      </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -3738,14 +3821,16 @@
       </c>
       <c r="K41"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>224</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="C42" s="4"/>
+      <c r="C42" s="41" t="s">
+        <v>224</v>
+      </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -3762,14 +3847,16 @@
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>230</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="C43" s="4"/>
+      <c r="C43" s="41" t="s">
+        <v>230</v>
+      </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -3786,14 +3873,16 @@
         <v>235</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>236</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C44" s="4"/>
+      <c r="C44" s="41" t="s">
+        <v>236</v>
+      </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -3810,14 +3899,16 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>242</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C45" s="4"/>
+      <c r="C45" s="41" t="s">
+        <v>242</v>
+      </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -3834,14 +3925,16 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="27.6">
+    <row r="46" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>248</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C46" s="4"/>
+      <c r="C46" s="41" t="s">
+        <v>248</v>
+      </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -3856,14 +3949,16 @@
         <v>252</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="13" customFormat="1" ht="96.6" customHeight="1">
+    <row r="47" spans="1:11" s="13" customFormat="1" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>253</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C47" s="4"/>
+      <c r="C47" s="41" t="s">
+        <v>253</v>
+      </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
@@ -3881,14 +3976,16 @@
       </c>
       <c r="K47"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>259</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C48" s="4"/>
+      <c r="C48" s="41" t="s">
+        <v>259</v>
+      </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
@@ -3905,14 +4002,16 @@
         <v>264</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>265</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C49" s="4"/>
+      <c r="C49" s="41" t="s">
+        <v>265</v>
+      </c>
       <c r="D49" s="40" t="s">
         <v>267</v>
       </c>
@@ -3935,7 +4034,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="55.15">
+    <row r="50" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>274</v>
       </c>
@@ -3943,573 +4042,575 @@
         <v>275</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>276</v>
+        <v>705</v>
       </c>
       <c r="D50" s="40"/>
       <c r="E50" s="40"/>
       <c r="F50" s="40"/>
       <c r="G50" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="H50" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="I50" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="I50" s="9" t="s">
+      <c r="J50" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="J50" s="9" t="s">
+      <c r="K50" s="13"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="K50" s="13"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="17" t="s">
+      <c r="B51" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>282</v>
-      </c>
       <c r="C51" s="4" t="s">
-        <v>276</v>
+        <v>705</v>
       </c>
       <c r="D51" s="40"/>
       <c r="E51" s="40"/>
       <c r="F51" s="40"/>
       <c r="G51" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="H51" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="H51" s="7" t="s">
+      <c r="I51" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="I51" s="9" t="s">
+      <c r="J51" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="J51" s="9" t="s">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="4" t="s">
-        <v>287</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
-        <v>276</v>
+        <v>705</v>
       </c>
       <c r="D52" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="G52" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="H52" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="H52" s="7" t="s">
+      <c r="I52" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="I52" s="9" t="s">
+      <c r="J52" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="J52" s="9" t="s">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="E53" s="33" t="s">
         <v>297</v>
       </c>
-      <c r="E53" s="33" t="s">
+      <c r="F53" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G53" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="G53" s="9" t="s">
+      <c r="H53" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="H53" s="7" t="s">
+      <c r="I53" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="I53" s="9" t="s">
+      <c r="J53" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="J53" s="9" t="s">
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="17" t="s">
+      <c r="B54" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="C54" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D54" s="4" t="s">
+      <c r="E54" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="F54" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="H54" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="H54" s="7" t="s">
+      <c r="I54" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="I54" s="9" t="s">
+      <c r="J54" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="J54" s="9" t="s">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="17" t="s">
+      <c r="B55" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D55" s="4" t="s">
+      <c r="E55" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="F55" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G55" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="G55" s="9" t="s">
+      <c r="H55" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="H55" s="7" t="s">
+      <c r="I55" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="I55" s="9" t="s">
+      <c r="J55" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="J55" s="9" t="s">
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="17" t="s">
+      <c r="B56" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D56" s="33" t="s">
         <v>321</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D56" s="33" t="s">
+      <c r="E56" s="33" t="s">
         <v>322</v>
       </c>
-      <c r="E56" s="33" t="s">
+      <c r="F56" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G56" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="F56" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="G56" s="9" t="s">
+      <c r="H56" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="H56" s="7" t="s">
+      <c r="I56" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="I56" s="9" t="s">
+      <c r="J56" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="J56" s="9" t="s">
+    </row>
+    <row r="57" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" ht="27.6">
-      <c r="A57" s="17" t="s">
+      <c r="B57" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>330</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="H57" s="7" t="s">
         <v>331</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>332</v>
       </c>
       <c r="I57" s="14"/>
       <c r="J57" s="14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="17" t="s">
+      <c r="B58" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="C58" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D58" s="4" t="s">
+      <c r="E58" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="F58" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G58" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="F58" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="G58" s="9" t="s">
+      <c r="H58" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="H58" s="7" t="s">
+      <c r="I58" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="I58" s="9" t="s">
+      <c r="J58" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="J58" s="9" t="s">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="A59" s="17" t="s">
+      <c r="B59" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D59" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="F59" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="J59" s="9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
         <v>345</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="H59" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I59" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="J59" s="9" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="27.6">
-      <c r="A60" s="17" t="s">
+      <c r="B60" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="7" t="s">
         <v>347</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>348</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="24" t="s">
+        <v>347</v>
+      </c>
+      <c r="G60" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="G60" s="10" t="s">
+      <c r="H60" s="7" t="s">
         <v>349</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>350</v>
       </c>
       <c r="I60" s="14"/>
       <c r="J60" s="14" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
         <v>351</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" s="17" t="s">
-        <v>352</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" s="4" t="s">
-        <v>276</v>
+        <v>705</v>
       </c>
       <c r="D61" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="F61" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G61" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="F61" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="G61" s="9" t="s">
+      <c r="H61" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="H61" s="7" t="s">
+      <c r="I61" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="I61" s="9" t="s">
+      <c r="J61" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="J61" s="9" t="s">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="17" t="s">
+      <c r="B62" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="D62" s="33" t="s">
         <v>361</v>
       </c>
-      <c r="D62" s="33" t="s">
+      <c r="E62" s="33" t="s">
         <v>362</v>
       </c>
-      <c r="E62" s="33" t="s">
+      <c r="F62" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="F62" s="35" t="s">
+      <c r="G62" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="H62" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="H62" s="7" t="s">
+      <c r="I62" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="I62" s="9" t="s">
+      <c r="J62" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="J62" s="9" t="s">
+    </row>
+    <row r="63" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="82.9">
-      <c r="A63" s="17" t="s">
+      <c r="B63" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="B63" s="23" t="s">
-        <v>370</v>
-      </c>
-      <c r="C63" s="4"/>
+      <c r="C63" s="4" t="s">
+        <v>705</v>
+      </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="H63" s="21" t="s">
         <v>371</v>
-      </c>
-      <c r="H63" s="21" t="s">
-        <v>372</v>
       </c>
       <c r="I63" s="14"/>
       <c r="J63" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="K63" s="13"/>
+    </row>
+    <row r="64" spans="1:11" ht="39" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="K63" s="13"/>
-    </row>
-    <row r="64" spans="1:11" ht="41.45">
-      <c r="A64" s="17" t="s">
+      <c r="B64" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="C64" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D64" s="4" t="s">
+      <c r="E64" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="F64" s="36" t="s">
         <v>377</v>
       </c>
-      <c r="F64" s="36" t="s">
+      <c r="G64" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="G64" s="9" t="s">
+      <c r="H64" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="H64" s="7" t="s">
+      <c r="I64" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="I64" s="9" t="s">
+      <c r="J64" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="J64" s="9" t="s">
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" s="17" t="s">
+      <c r="B65" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="C65" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D65" s="33" t="s">
         <v>384</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D65" s="33" t="s">
+      <c r="E65" s="33" t="s">
         <v>385</v>
       </c>
-      <c r="E65" s="33" t="s">
+      <c r="F65" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="G65" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="G65" s="9" t="s">
+      <c r="H65" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="H65" s="7" t="s">
+      <c r="I65" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="I65" s="9" t="s">
+      <c r="J65" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="J65" s="9" t="s">
+    </row>
+    <row r="66" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="41.45">
-      <c r="A66" s="17" t="s">
+      <c r="B66" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="F66" s="37" t="s">
         <v>392</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="F66" s="37" t="s">
+      <c r="G66" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="H66" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="H66" s="7" t="s">
+      <c r="I66" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="I66" s="9" t="s">
+      <c r="J66" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="J66" s="9" t="s">
+    </row>
+    <row r="67" spans="1:10" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" ht="55.15">
-      <c r="A67" s="17" t="s">
+      <c r="B67" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="C67" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D67" s="34" t="s">
         <v>399</v>
       </c>
-      <c r="C67" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D67" s="34" t="s">
+      <c r="E67" s="34" t="s">
         <v>400</v>
       </c>
-      <c r="E67" s="34" t="s">
+      <c r="F67" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="G67" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="F67" s="38" t="s">
-        <v>387</v>
-      </c>
-      <c r="G67" s="9" t="s">
+      <c r="H67" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="H67" s="7" t="s">
+      <c r="I67" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="I67" s="9" t="s">
+      <c r="J67" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
         <v>404</v>
       </c>
-      <c r="J67" s="9" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" s="17" t="s">
+      <c r="B68" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="C68" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D68" s="33" t="s">
         <v>406</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D68" s="33" t="s">
+      <c r="E68" s="33" t="s">
         <v>407</v>
       </c>
-      <c r="E68" s="33" t="s">
+      <c r="F68" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="G68" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="F68" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="G68" s="9" t="s">
+      <c r="H68" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="H68" s="7" t="s">
+      <c r="I68" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="I68" s="9" t="s">
-        <v>411</v>
-      </c>
       <c r="J68" s="9" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="33"/>
       <c r="H69"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="33"/>
       <c r="H70"/>
     </row>
@@ -4534,13 +4635,13 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E48" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E64" sqref="E64"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -4549,1228 +4650,1228 @@
     <col min="5" max="5" width="127.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" t="s">
         <v>412</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>413</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>414</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>415</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>417</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>418</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>419</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>420</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>422</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3" t="s">
         <v>423</v>
       </c>
-      <c r="C3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>424</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>426</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D4" t="s">
         <v>427</v>
       </c>
-      <c r="C4" t="s">
-        <v>419</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>428</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>430</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>418</v>
+      </c>
+      <c r="D5" t="s">
         <v>431</v>
       </c>
-      <c r="C5" t="s">
-        <v>419</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>432</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>434</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>435</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>436</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>437</v>
       </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>439</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>435</v>
+      </c>
+      <c r="D7" t="s">
         <v>440</v>
       </c>
-      <c r="C7" t="s">
-        <v>436</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>441</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>443</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>435</v>
+      </c>
+      <c r="D8" t="s">
         <v>444</v>
       </c>
-      <c r="C8" t="s">
-        <v>436</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>445</v>
       </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>447</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>435</v>
+      </c>
+      <c r="D9" t="s">
         <v>448</v>
       </c>
-      <c r="C9" t="s">
-        <v>436</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>449</v>
       </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>451</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>435</v>
+      </c>
+      <c r="D10" t="s">
         <v>452</v>
       </c>
-      <c r="C10" t="s">
-        <v>436</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>453</v>
       </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>455</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>435</v>
+      </c>
+      <c r="D11" t="s">
         <v>456</v>
       </c>
-      <c r="C11" t="s">
-        <v>436</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>457</v>
       </c>
-      <c r="E11" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>459</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>435</v>
+      </c>
+      <c r="D12" t="s">
         <v>460</v>
       </c>
-      <c r="C12" t="s">
-        <v>436</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>461</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>463</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>464</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>465</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>466</v>
       </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>468</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>464</v>
+      </c>
+      <c r="D14" t="s">
         <v>469</v>
       </c>
-      <c r="C14" t="s">
-        <v>465</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>470</v>
       </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>472</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>464</v>
+      </c>
+      <c r="D15" t="s">
         <v>473</v>
       </c>
-      <c r="C15" t="s">
-        <v>465</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>474</v>
       </c>
-      <c r="E15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>476</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>464</v>
+      </c>
+      <c r="D16" t="s">
         <v>477</v>
       </c>
-      <c r="C16" t="s">
-        <v>465</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>478</v>
       </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>480</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>464</v>
+      </c>
+      <c r="D17" t="s">
         <v>481</v>
       </c>
-      <c r="C17" t="s">
-        <v>465</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>482</v>
       </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>484</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>464</v>
+      </c>
+      <c r="D18" t="s">
         <v>485</v>
       </c>
-      <c r="C18" t="s">
-        <v>465</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>486</v>
       </c>
-      <c r="E18" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>488</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>464</v>
+      </c>
+      <c r="D19" t="s">
         <v>489</v>
       </c>
-      <c r="C19" t="s">
-        <v>465</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>490</v>
       </c>
-      <c r="E19" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>492</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>464</v>
+      </c>
+      <c r="D20" t="s">
         <v>493</v>
       </c>
-      <c r="C20" t="s">
-        <v>465</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>494</v>
       </c>
-      <c r="E20" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>496</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>464</v>
+      </c>
+      <c r="D21" t="s">
         <v>497</v>
       </c>
-      <c r="C21" t="s">
-        <v>465</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>498</v>
       </c>
-      <c r="E21" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>500</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>464</v>
+      </c>
+      <c r="D22" t="s">
         <v>501</v>
       </c>
-      <c r="C22" t="s">
-        <v>465</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>502</v>
       </c>
-      <c r="E22" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>504</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>464</v>
+      </c>
+      <c r="D23" t="s">
         <v>505</v>
       </c>
-      <c r="C23" t="s">
-        <v>465</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>506</v>
       </c>
-      <c r="E23" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>508</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>464</v>
+      </c>
+      <c r="D24" t="s">
         <v>509</v>
       </c>
-      <c r="C24" t="s">
-        <v>465</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>510</v>
       </c>
-      <c r="E24" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>512</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>464</v>
+      </c>
+      <c r="D25" t="s">
         <v>513</v>
       </c>
-      <c r="C25" t="s">
-        <v>465</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>514</v>
       </c>
-      <c r="E25" t="s">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>516</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>464</v>
+      </c>
+      <c r="D26" t="s">
         <v>517</v>
       </c>
-      <c r="C26" t="s">
-        <v>465</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>518</v>
       </c>
-      <c r="E26" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>520</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>464</v>
+      </c>
+      <c r="D27" t="s">
         <v>521</v>
       </c>
-      <c r="C27" t="s">
-        <v>465</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>522</v>
       </c>
-      <c r="E27" t="s">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>524</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>464</v>
+      </c>
+      <c r="D28" t="s">
         <v>525</v>
       </c>
-      <c r="C28" t="s">
-        <v>465</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>526</v>
       </c>
-      <c r="E28" t="s">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>528</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>529</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>530</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>531</v>
       </c>
-      <c r="E29" t="s">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>533</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>529</v>
+      </c>
+      <c r="D30" t="s">
         <v>534</v>
       </c>
-      <c r="C30" t="s">
-        <v>530</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>535</v>
       </c>
-      <c r="E30" t="s">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>537</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>529</v>
+      </c>
+      <c r="D31" t="s">
         <v>538</v>
       </c>
-      <c r="C31" t="s">
-        <v>530</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>539</v>
       </c>
-      <c r="E31" t="s">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>541</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>529</v>
+      </c>
+      <c r="D32" t="s">
         <v>542</v>
       </c>
-      <c r="C32" t="s">
-        <v>530</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>543</v>
       </c>
-      <c r="E32" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
         <v>545</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>546</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>547</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>548</v>
       </c>
-      <c r="E33" t="s">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>550</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>546</v>
+      </c>
+      <c r="D34" t="s">
         <v>551</v>
       </c>
-      <c r="C34" t="s">
-        <v>547</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>552</v>
       </c>
-      <c r="E34" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>554</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>546</v>
+      </c>
+      <c r="D35" t="s">
         <v>555</v>
       </c>
-      <c r="C35" t="s">
-        <v>547</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>556</v>
       </c>
-      <c r="E35" t="s">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
         <v>558</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>546</v>
+      </c>
+      <c r="D36" t="s">
         <v>559</v>
       </c>
-      <c r="C36" t="s">
-        <v>547</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>560</v>
       </c>
-      <c r="E36" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>562</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>563</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>564</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>565</v>
       </c>
-      <c r="E37" t="s">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>567</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>563</v>
+      </c>
+      <c r="D38" t="s">
         <v>568</v>
       </c>
-      <c r="C38" t="s">
-        <v>564</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>569</v>
       </c>
-      <c r="E38" t="s">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>571</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>563</v>
+      </c>
+      <c r="D39" t="s">
         <v>572</v>
       </c>
-      <c r="C39" t="s">
-        <v>564</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>573</v>
       </c>
-      <c r="E39" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>575</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>563</v>
+      </c>
+      <c r="D40" t="s">
         <v>576</v>
       </c>
-      <c r="C40" t="s">
-        <v>564</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>577</v>
       </c>
-      <c r="E40" t="s">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>579</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>563</v>
+      </c>
+      <c r="D41" t="s">
         <v>580</v>
       </c>
-      <c r="C41" t="s">
-        <v>564</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>581</v>
       </c>
-      <c r="E41" t="s">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>583</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
+        <v>563</v>
+      </c>
+      <c r="D42" t="s">
         <v>584</v>
       </c>
-      <c r="C42" t="s">
-        <v>564</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>585</v>
       </c>
-      <c r="E42" t="s">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>587</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>563</v>
+      </c>
+      <c r="D43" t="s">
         <v>588</v>
       </c>
-      <c r="C43" t="s">
-        <v>564</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>589</v>
       </c>
-      <c r="E43" t="s">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>591</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
+        <v>563</v>
+      </c>
+      <c r="D44" t="s">
         <v>592</v>
       </c>
-      <c r="C44" t="s">
-        <v>564</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>593</v>
       </c>
-      <c r="E44" t="s">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>595</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
+        <v>563</v>
+      </c>
+      <c r="D45" t="s">
         <v>596</v>
       </c>
-      <c r="C45" t="s">
-        <v>564</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>597</v>
       </c>
-      <c r="E45" t="s">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
         <v>599</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>563</v>
+      </c>
+      <c r="D46" t="s">
         <v>600</v>
       </c>
-      <c r="C46" t="s">
-        <v>564</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>601</v>
       </c>
-      <c r="E46" t="s">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>603</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
+        <v>563</v>
+      </c>
+      <c r="D47" t="s">
         <v>604</v>
       </c>
-      <c r="C47" t="s">
-        <v>564</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>605</v>
       </c>
-      <c r="E47" t="s">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>607</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
+        <v>563</v>
+      </c>
+      <c r="D48" t="s">
         <v>608</v>
       </c>
-      <c r="C48" t="s">
-        <v>564</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>609</v>
       </c>
-      <c r="E48" t="s">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
         <v>611</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
+        <v>563</v>
+      </c>
+      <c r="D49" t="s">
         <v>612</v>
       </c>
-      <c r="C49" t="s">
-        <v>564</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>613</v>
       </c>
-      <c r="E49" t="s">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
         <v>615</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
+        <v>563</v>
+      </c>
+      <c r="D50" t="s">
         <v>616</v>
       </c>
-      <c r="C50" t="s">
-        <v>564</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>617</v>
       </c>
-      <c r="E50" t="s">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
         <v>619</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
+        <v>563</v>
+      </c>
+      <c r="D51" t="s">
         <v>620</v>
       </c>
-      <c r="C51" t="s">
-        <v>564</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>621</v>
       </c>
-      <c r="E51" t="s">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
         <v>623</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>624</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>625</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>626</v>
       </c>
-      <c r="E52" t="s">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
         <v>628</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
+        <v>624</v>
+      </c>
+      <c r="D53" t="s">
         <v>629</v>
       </c>
-      <c r="C53" t="s">
-        <v>625</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>630</v>
       </c>
-      <c r="E53" t="s">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>627</v>
+      </c>
+      <c r="B54" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="s">
-        <v>628</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
+        <v>624</v>
+      </c>
+      <c r="D54" t="s">
         <v>632</v>
       </c>
-      <c r="C54" t="s">
-        <v>625</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>633</v>
       </c>
-      <c r="E54" t="s">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
         <v>635</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>624</v>
+      </c>
+      <c r="D55" t="s">
         <v>636</v>
       </c>
-      <c r="C55" t="s">
-        <v>625</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>637</v>
       </c>
-      <c r="E55" t="s">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
         <v>639</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>624</v>
+      </c>
+      <c r="D56" t="s">
         <v>640</v>
       </c>
-      <c r="C56" t="s">
-        <v>625</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>641</v>
       </c>
-      <c r="E56" t="s">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
         <v>643</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
+        <v>624</v>
+      </c>
+      <c r="D57" t="s">
         <v>644</v>
       </c>
-      <c r="C57" t="s">
-        <v>625</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>645</v>
       </c>
-      <c r="E57" t="s">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
+      <c r="B58" t="s">
         <v>647</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>648</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>649</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>650</v>
       </c>
-      <c r="E58" t="s">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
         <v>652</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>648</v>
+      </c>
+      <c r="D59" t="s">
         <v>653</v>
       </c>
-      <c r="C59" t="s">
-        <v>649</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>654</v>
       </c>
-      <c r="E59" t="s">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
+      <c r="B60" t="s">
         <v>656</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
+        <v>648</v>
+      </c>
+      <c r="D60" t="s">
+        <v>653</v>
+      </c>
+      <c r="E60" t="s">
         <v>657</v>
       </c>
-      <c r="C60" t="s">
-        <v>649</v>
-      </c>
-      <c r="D60" t="s">
-        <v>654</v>
-      </c>
-      <c r="E60" t="s">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" t="s">
+      <c r="B61" t="s">
         <v>659</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
+        <v>648</v>
+      </c>
+      <c r="D61" t="s">
+        <v>653</v>
+      </c>
+      <c r="E61" t="s">
         <v>660</v>
       </c>
-      <c r="C61" t="s">
-        <v>649</v>
-      </c>
-      <c r="D61" t="s">
-        <v>654</v>
-      </c>
-      <c r="E61" t="s">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" t="s">
+      <c r="B62" t="s">
         <v>662</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
+        <v>648</v>
+      </c>
+      <c r="D62" t="s">
         <v>663</v>
       </c>
-      <c r="C62" t="s">
-        <v>649</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>664</v>
       </c>
-      <c r="E62" t="s">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" t="s">
+      <c r="B63" t="s">
         <v>666</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
+        <v>648</v>
+      </c>
+      <c r="D63" t="s">
         <v>667</v>
       </c>
-      <c r="C63" t="s">
-        <v>649</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>668</v>
       </c>
-      <c r="E63" t="s">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" t="s">
+      <c r="B64" t="s">
         <v>670</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
+        <v>648</v>
+      </c>
+      <c r="D64" t="s">
         <v>671</v>
       </c>
-      <c r="C64" t="s">
-        <v>649</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>672</v>
       </c>
-      <c r="E64" t="s">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
+      <c r="B65" t="s">
         <v>674</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
+        <v>648</v>
+      </c>
+      <c r="D65" t="s">
         <v>675</v>
       </c>
-      <c r="C65" t="s">
-        <v>649</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>676</v>
       </c>
-      <c r="E65" t="s">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
+      <c r="B66" t="s">
         <v>678</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>648</v>
+      </c>
+      <c r="D66" t="s">
         <v>679</v>
       </c>
-      <c r="C66" t="s">
-        <v>649</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>680</v>
       </c>
-      <c r="E66" t="s">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
+      <c r="B67" t="s">
         <v>682</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>648</v>
+      </c>
+      <c r="D67" t="s">
         <v>683</v>
       </c>
-      <c r="C67" t="s">
-        <v>649</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>684</v>
       </c>
-      <c r="E67" t="s">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" t="s">
+      <c r="B68" t="s">
         <v>686</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
+        <v>648</v>
+      </c>
+      <c r="D68" t="s">
         <v>687</v>
       </c>
-      <c r="C68" t="s">
-        <v>649</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>688</v>
       </c>
-      <c r="E68" t="s">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
+      <c r="B69" t="s">
         <v>690</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
+        <v>648</v>
+      </c>
+      <c r="D69" t="s">
         <v>691</v>
       </c>
-      <c r="C69" t="s">
-        <v>649</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>692</v>
       </c>
-      <c r="E69" t="s">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" t="s">
+      <c r="B70" t="s">
         <v>694</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>648</v>
+      </c>
+      <c r="D70" t="s">
         <v>695</v>
       </c>
-      <c r="C70" t="s">
-        <v>649</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>696</v>
       </c>
-      <c r="E70" t="s">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" t="s">
+      <c r="B71" t="s">
         <v>698</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
+        <v>648</v>
+      </c>
+      <c r="D71" t="s">
         <v>699</v>
       </c>
-      <c r="C71" t="s">
-        <v>649</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>700</v>
       </c>
-      <c r="E71" t="s">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" t="s">
+      <c r="B72" t="s">
         <v>702</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
+        <v>648</v>
+      </c>
+      <c r="D72" t="s">
         <v>703</v>
       </c>
-      <c r="C72" t="s">
-        <v>649</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>704</v>
-      </c>
-      <c r="E72" t="s">
-        <v>705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>